<commit_message>
calc couple in inverted index
</commit_message>
<xml_diff>
--- a/hammer-project/hammer-shark/data_us/1_result.xlsx
+++ b/hammer-project/hammer-shark/data_us/1_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="34400" yWindow="-11240" windowWidth="25600" windowHeight="14480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_1000" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="56">
   <si>
     <t>Test 1</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>SPARK v2</t>
+  </si>
+  <si>
+    <t>couple</t>
   </si>
 </sst>
 </file>
@@ -700,7 +703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -716,6 +721,12 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2">
+        <v>127396</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -2495,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2512,6 +2523,12 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="17">
+        <v>1105390</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -4245,8 +4262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J53" sqref="J53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4259,6 +4276,12 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2">
+        <v>1794330</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>